<commit_message>
updated script_dependents with rsync script
</commit_message>
<xml_diff>
--- a/dependencies/brucella/abortus1/script_dependents/script2/RemoveFromAnalysis.xlsx
+++ b/dependencies/brucella/abortus1/script_dependents/script2/RemoveFromAnalysis.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/root/TStuber/Results/brucella/abortus1/script_dependents/python/script2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\TStuber\Results\brucella\abortus1\script_dependents\script2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="65640" yWindow="9960" windowWidth="22260" windowHeight="16920" tabRatio="500"/>
+    <workbookView xWindow="28935" yWindow="9960" windowWidth="22260" windowHeight="16920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>B82-2330-Broad</t>
   </si>
@@ -59,12 +56,6 @@
     <t>B10-1034</t>
   </si>
   <si>
-    <t>B10-0943</t>
-  </si>
-  <si>
-    <t>B12-0557</t>
-  </si>
-  <si>
     <t>B12-0393-2</t>
   </si>
   <si>
@@ -102,6 +93,21 @@
   </si>
   <si>
     <t>B16-0120-S1</t>
+  </si>
+  <si>
+    <t>2308_GCA_000054005-2</t>
+  </si>
+  <si>
+    <t>B17-0712</t>
+  </si>
+  <si>
+    <t>B17-0712-RETRO</t>
+  </si>
+  <si>
+    <t>B17-0712-SMAM</t>
+  </si>
+  <si>
+    <t>B17-0712-TRACH</t>
   </si>
 </sst>
 </file>
@@ -148,6 +154,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -416,137 +425,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2002734562</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>